<commit_message>
Updated Project Plan CYRS versioning Review CRS Added to the input Documents Signed-off-by: ahmed.zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Software components/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Software components/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\Software components\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC28F6C-0154-43F9-B7EA-3C5AF9D3712B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5195EBA-80C2-488B-964A-50B3DF08D1AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,6 +357,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,8 +630,8 @@
   <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -965,12 +968,14 @@
         <v>43852</v>
       </c>
       <c r="G9" s="20">
-        <v>43852</v>
+        <v>43854</v>
       </c>
       <c r="H9" s="20">
-        <v>43853</v>
+        <v>43854</v>
       </c>
-      <c r="I9" s="17"/>
+      <c r="I9" s="33">
+        <v>1</v>
+      </c>
       <c r="J9" s="17" t="s">
         <v>26</v>
       </c>
@@ -1015,7 +1020,7 @@
         <v>43854</v>
       </c>
       <c r="G10" s="20">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="17"/>
@@ -1063,12 +1068,14 @@
         <v>43854</v>
       </c>
       <c r="G11" s="20">
-        <v>43852</v>
+        <v>43854</v>
       </c>
       <c r="H11" s="20">
         <v>43854</v>
       </c>
-      <c r="I11" s="17"/>
+      <c r="I11" s="33">
+        <v>1</v>
+      </c>
       <c r="J11" s="17" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Signed-off-by: Nafe3 <eng.mohamed.nafe3@gmail.com> (#6)
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Software components/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Software components/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\Software components\SW deliveries log\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Subjects\Software Engineering\26-1-2020\Digital_Elevator_PO4_DGELV\Software components\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250FC42A-5213-4F02-A3A3-7942FB60E3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A749FD-39D0-46FE-A51C-0CB296173314}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO4_DGELV_Project_Plan" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -333,21 +333,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -357,6 +348,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,24 +620,24 @@
   </sheetPr>
   <dimension ref="A1:AF1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" customWidth="1"/>
-    <col min="11" max="11" width="50.453125" customWidth="1"/>
-    <col min="12" max="12" width="3.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="50.44140625" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
     <col min="13" max="32" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,11 +688,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="25"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -733,11 +727,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -767,11 +761,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -795,8 +789,8 @@
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -958,22 +952,22 @@
       <c r="D9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="30">
         <v>43851</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="30">
         <v>43852</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="30">
         <v>43854</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="30">
         <v>43854</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="18">
         <v>3</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="18" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="17"/>
@@ -1010,22 +1004,22 @@
       <c r="D10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="30">
         <v>43852</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="30">
         <v>43854</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="30">
         <v>43854</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="30">
         <v>43855</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="18">
         <v>3</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="18" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="17"/>
@@ -1062,22 +1056,22 @@
       <c r="D11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="30">
         <v>43852</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="30">
         <v>43854</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="30">
         <v>43854</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="30">
         <v>43854</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="18">
         <v>2</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="18" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="17"/>
@@ -1114,16 +1108,16 @@
       <c r="D12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="30">
         <v>43852</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="30">
         <v>43854</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17" t="s">
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="17"/>
@@ -1160,19 +1154,19 @@
       <c r="D13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="30">
         <v>43855</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="30">
         <v>43856</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="30">
         <v>43855</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="30">
         <v>43855</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="18">
         <v>1</v>
       </c>
       <c r="J13" s="18" t="s">
@@ -1212,19 +1206,19 @@
       <c r="D14" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="30">
         <v>43854</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="30">
         <v>43855</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="30">
         <v>43854</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="30">
         <v>43855</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="18">
         <v>1</v>
       </c>
       <c r="J14" s="18" t="s">
@@ -1264,14 +1258,14 @@
       <c r="D15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="30">
         <v>43855</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="30">
         <v>43856</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18" t="s">
         <v>19</v>
@@ -1369,9 +1363,9 @@
     </row>
     <row r="18" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1403,9 +1397,9 @@
     </row>
     <row r="19" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1437,8 +1431,8 @@
     </row>
     <row r="20" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1471,8 +1465,8 @@
     </row>
     <row r="21" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1505,8 +1499,8 @@
     </row>
     <row r="22" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1539,9 +1533,9 @@
     </row>
     <row r="23" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1573,9 +1567,9 @@
     </row>
     <row r="24" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="23"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1607,9 +1601,9 @@
     </row>
     <row r="25" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="24"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -34876,10 +34870,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" orientation="landscape"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C000000Gantt Chart_x000D_</oddHeader>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Project Plan Signed-off-by: ahmed.zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Software components/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Software components/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\Software components\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250FC42A-5213-4F02-A3A3-7942FB60E3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC30385-BF42-450E-89A7-D59FC8D19A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Sara Youssif</t>
+  </si>
+  <si>
+    <t>SRS Document Update</t>
   </si>
 </sst>
 </file>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -348,6 +351,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -624,11 +629,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF1002"/>
+  <dimension ref="A1:AF1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,11 +699,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -733,11 +738,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -767,11 +772,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -795,8 +800,8 @@
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1120,11 +1125,17 @@
       <c r="F12" s="20">
         <v>43854</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="17"/>
+      <c r="G12" s="20">
+        <v>43855</v>
+      </c>
+      <c r="H12" s="20">
+        <v>43856</v>
+      </c>
+      <c r="I12" s="25">
+        <v>2</v>
+      </c>
       <c r="J12" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="K12" s="17"/>
       <c r="L12" s="3"/>
@@ -1270,11 +1281,17 @@
       <c r="F15" s="20">
         <v>43856</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="18"/>
+      <c r="G15" s="20">
+        <v>43855</v>
+      </c>
+      <c r="H15" s="20">
+        <v>43855</v>
+      </c>
+      <c r="I15" s="25">
+        <v>1</v>
+      </c>
       <c r="J15" s="18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="3"/>
@@ -1299,18 +1316,30 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="5"/>
     </row>
-    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+    <row r="16" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="20">
+        <v>43858</v>
+      </c>
+      <c r="F16" s="20">
+        <v>43860</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="18"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1369,9 +1398,9 @@
     </row>
     <row r="18" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1439,7 +1468,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1541,7 +1570,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1609,7 +1638,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="24"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1641,9 +1670,9 @@
     </row>
     <row r="26" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2047,73 +2076,73 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="5"/>
     </row>
-    <row r="38" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-    </row>
-    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="5"/>
+    </row>
+    <row r="39" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="3"/>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="5"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
     </row>
     <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -8339,37 +8368,37 @@
     </row>
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
-      <c r="G223" s="1"/>
-      <c r="H223" s="1"/>
-      <c r="I223" s="1"/>
-      <c r="J223" s="1"/>
-      <c r="K223" s="1"/>
-      <c r="L223" s="1"/>
-      <c r="M223" s="1"/>
-      <c r="N223" s="1"/>
-      <c r="O223" s="1"/>
-      <c r="P223" s="1"/>
-      <c r="Q223" s="1"/>
-      <c r="R223" s="1"/>
-      <c r="S223" s="1"/>
-      <c r="T223" s="1"/>
-      <c r="U223" s="1"/>
-      <c r="V223" s="1"/>
-      <c r="W223" s="1"/>
-      <c r="X223" s="1"/>
-      <c r="Y223" s="1"/>
-      <c r="Z223" s="1"/>
-      <c r="AA223" s="1"/>
-      <c r="AB223" s="1"/>
-      <c r="AC223" s="1"/>
-      <c r="AD223" s="1"/>
-      <c r="AE223" s="1"/>
-      <c r="AF223" s="1"/>
+      <c r="B223" s="3"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="3"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="3"/>
+      <c r="K223" s="3"/>
+      <c r="L223" s="3"/>
+      <c r="M223" s="3"/>
+      <c r="N223" s="3"/>
+      <c r="O223" s="3"/>
+      <c r="P223" s="3"/>
+      <c r="Q223" s="3"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="3"/>
+      <c r="T223" s="3"/>
+      <c r="U223" s="3"/>
+      <c r="V223" s="3"/>
+      <c r="W223" s="3"/>
+      <c r="X223" s="3"/>
+      <c r="Y223" s="3"/>
+      <c r="Z223" s="3"/>
+      <c r="AA223" s="3"/>
+      <c r="AB223" s="3"/>
+      <c r="AC223" s="3"/>
+      <c r="AD223" s="3"/>
+      <c r="AE223" s="3"/>
+      <c r="AF223" s="5"/>
     </row>
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
@@ -34857,6 +34886,40 @@
       <c r="AE1002" s="1"/>
       <c r="AF1002" s="1"/>
     </row>
+    <row r="1003" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+      <c r="AA1003" s="1"/>
+      <c r="AB1003" s="1"/>
+      <c r="AC1003" s="1"/>
+      <c r="AD1003" s="1"/>
+      <c r="AE1003" s="1"/>
+      <c r="AF1003" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G2:K4"/>
@@ -34868,10 +34931,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C9:C15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C9:C16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J9:J15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J9:J16" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>